<commit_message>
new changes made on multiple pages and also new pages added
</commit_message>
<xml_diff>
--- a/public/excelTemplate.xlsx
+++ b/public/excelTemplate.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>Device</t>
-  </si>
-  <si>
-    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -416,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,7 +432,7 @@
     <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,11 +457,8 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -489,11 +483,8 @@
       <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -518,13 +509,10 @@
       <c r="H3" t="s">
         <v>14</v>
       </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -546,9 +534,6 @@
       </c>
       <c r="H4" t="s">
         <v>19</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>